<commit_message>
made changes for cloud aws ec2 instance in jenkins
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1125" windowWidth="18615" windowHeight="7020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1125" windowWidth="18045" windowHeight="5265" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -503,7 +504,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -514,11 +515,12 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
     <col min="10" max="10" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>